<commit_message>
email db sync done with validation
</commit_message>
<xml_diff>
--- a/constants/dummyData/students.xlsx
+++ b/constants/dummyData/students.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Jordan Miller</t>
   </si>
   <si>
-    <t xml:space="preserve">anthonywalker@example.com</t>
+    <t xml:space="preserve">alanwalker23@example.net</t>
   </si>
   <si>
     <t xml:space="preserve">Roberto Johnson</t>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">zjacobs@example.org</t>
   </si>
   <si>
-    <t xml:space="preserve">Justin Carroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ysutton@example.net</t>
+    <t xml:space="preserve">Justin Creamroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kirky@example.com</t>
   </si>
   <si>
     <t xml:space="preserve">Kirk Johnson</t>
@@ -329,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -351,6 +351,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -395,8 +401,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,12 +430,13 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="A7:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,8 +447,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -476,7 +487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -484,15 +495,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
@@ -500,7 +511,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -508,7 +519,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -516,7 +527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -524,7 +535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
@@ -532,7 +543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
@@ -540,7 +551,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>28</v>
       </c>
@@ -548,7 +559,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
@@ -556,7 +567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>32</v>
       </c>
@@ -564,7 +575,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>34</v>
       </c>
@@ -572,7 +583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>36</v>
       </c>
@@ -580,7 +591,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>38</v>
       </c>
@@ -588,7 +599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>40</v>
       </c>
@@ -596,7 +607,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>42</v>
       </c>
@@ -604,7 +615,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
@@ -612,7 +623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
@@ -620,7 +631,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>48</v>
       </c>
@@ -628,7 +639,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>50</v>
       </c>
@@ -636,7 +647,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>52</v>
       </c>
@@ -644,7 +655,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>54</v>
       </c>
@@ -652,7 +663,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>56</v>
       </c>
@@ -660,7 +671,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>58</v>
       </c>
@@ -668,7 +679,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>60</v>
       </c>
@@ -676,7 +687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>62</v>
       </c>
@@ -684,7 +695,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>64</v>
       </c>
@@ -692,7 +703,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>66</v>
       </c>
@@ -700,7 +711,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>68</v>
       </c>
@@ -708,7 +719,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>70</v>
       </c>
@@ -716,7 +727,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>72</v>
       </c>
@@ -724,7 +735,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>74</v>
       </c>
@@ -732,7 +743,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>76</v>
       </c>
@@ -740,7 +751,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>78</v>
       </c>
@@ -748,7 +759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>80</v>
       </c>
@@ -756,7 +767,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>82</v>
       </c>
@@ -764,7 +775,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>84</v>
       </c>
@@ -772,7 +783,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>86</v>
       </c>
@@ -780,7 +791,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>88</v>
       </c>
@@ -788,7 +799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>90</v>
       </c>
@@ -796,7 +807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>92</v>
       </c>
@@ -804,7 +815,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>94</v>
       </c>
@@ -812,7 +823,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>96</v>
       </c>
@@ -820,7 +831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>98</v>
       </c>

</xml_diff>